<commit_message>
Add Pytest and Webscraping practice
</commit_message>
<xml_diff>
--- a/WebScraping/Mukesh/Report.xlsx
+++ b/WebScraping/Mukesh/Report.xlsx
@@ -22,6 +22,7 @@
   <fonts count="5">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -42,6 +43,7 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="1"/>
       <sz val="10"/>
@@ -74,11 +76,14 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -288,65 +293,65 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1" ht="39" customHeight="1" s="2">
-      <c r="A1" s="3" t="inlineStr">
+    <row r="1" ht="39" customHeight="1" s="3">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Number</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" s="2">
-      <c r="A2" s="4" t="inlineStr">
+    <row r="2" ht="12.8" customHeight="1" s="3">
+      <c r="A2" s="5" t="inlineStr">
         <is>
           <t>Jimi</t>
         </is>
       </c>
-      <c r="B2" s="4" t="inlineStr">
+      <c r="B2" s="5" t="inlineStr">
         <is>
           <t>Chicago</t>
         </is>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C2" s="5" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="3" ht="12.8" customHeight="1" s="2">
-      <c r="A3" s="4" t="inlineStr">
+    <row r="3" ht="12.8" customHeight="1" s="3">
+      <c r="A3" s="5" t="inlineStr">
         <is>
           <t>Hendrix</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" s="5" t="inlineStr">
         <is>
           <t>Boston</t>
         </is>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="5" t="n">
         <v>60</v>
       </c>
     </row>
-    <row r="4" ht="12.8" customHeight="1" s="2">
-      <c r="A4" s="4" t="inlineStr">
+    <row r="4" ht="12.8" customHeight="1" s="3">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>Python</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
+      <c r="B4" s="5" t="inlineStr">
         <is>
           <t>Maine</t>
         </is>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="5" t="n">
         <v>99</v>
       </c>
     </row>
@@ -394,35 +399,35 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="2">
-      <c r="A1" s="3" t="inlineStr">
+    <row r="1" ht="12.8" customHeight="1" s="3">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Number</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" s="2">
-      <c r="A2" s="4" t="inlineStr">
+    <row r="2" ht="12.8" customHeight="1" s="3">
+      <c r="A2" s="5" t="inlineStr">
         <is>
           <t>John</t>
         </is>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="5" t="n">
         <v>90.05</v>
       </c>
     </row>
-    <row r="3" ht="12.8" customHeight="1" s="2">
-      <c r="A3" s="4" t="inlineStr">
+    <row r="3" ht="12.8" customHeight="1" s="3">
+      <c r="A3" s="5" t="inlineStr">
         <is>
           <t>Peter</t>
         </is>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="5" t="n">
         <v>91.09999999999999</v>
       </c>
     </row>

</xml_diff>